<commit_message>
Programa Correcto y Funcional (falta test ANOVA)
</commit_message>
<xml_diff>
--- a/excel_template.xlsx
+++ b/excel_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Desktop\Pablo\ING.Biomedica (UPM)\4.Curso\(LSB) Laboratorio de Señales Biomedicas\Practicas\Practica 2\Ratones Tratados (Vehiculo)\LSB-P2-analyzer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Desktop\Pablo\ING.Biomedica (UPM)\4.Curso\(LSB) Laboratorio de Señales Biomedicas\Practicas\Practica 2\datos-txt&amp;analisis\LSB-P2-analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422A18E9-B967-409E-9CCB-11DB422969EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F821BD-968B-4C31-A277-9F261E26D111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="984" yWindow="348" windowWidth="21600" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>AMPLITUD</t>
   </si>
@@ -48,9 +48,6 @@
     <t>HI</t>
   </si>
   <si>
-    <t>RATON 1</t>
-  </si>
-  <si>
     <t>BASAL</t>
   </si>
   <si>
@@ -60,15 +57,6 @@
     <t>2 SEMANAS</t>
   </si>
   <si>
-    <t>RATON2</t>
-  </si>
-  <si>
-    <t>RATON 3</t>
-  </si>
-  <si>
-    <t>RATON 4</t>
-  </si>
-  <si>
     <t>MEDIA BASAL</t>
   </si>
   <si>
@@ -87,14 +75,59 @@
     <t>DESVIACION-2 SEMANAS</t>
   </si>
   <si>
-    <t>Correlación de Pearson</t>
+    <t>R</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>CORRELACIÓN DE PEARSON</t>
+  </si>
+  <si>
+    <t>RATÓN 1</t>
+  </si>
+  <si>
+    <t>RATÓN2</t>
+  </si>
+  <si>
+    <t>RATÓN 3</t>
+  </si>
+  <si>
+    <t>RATÓN 4</t>
+  </si>
+  <si>
+    <r>
+      <t>Nvl Significancia  (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>α</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,8 +165,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,8 +218,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -517,8 +562,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
@@ -526,22 +604,20 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -620,48 +696,121 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="28" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="14" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="40% - Énfasis2" xfId="2" builtinId="35"/>
     <cellStyle name="40% - Énfasis4" xfId="4" builtinId="43"/>
+    <cellStyle name="40% - Énfasis5" xfId="8" builtinId="47"/>
     <cellStyle name="40% - Énfasis6" xfId="6" builtinId="51"/>
     <cellStyle name="Énfasis2" xfId="1" builtinId="33"/>
     <cellStyle name="Énfasis4" xfId="3" builtinId="41"/>
     <cellStyle name="Énfasis6" xfId="5" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -979,402 +1128,486 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" customWidth="1"/>
+    <col min="12" max="12" width="31.77734375" customWidth="1"/>
+    <col min="13" max="13" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="41" t="s">
+      <c r="D2" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="52"/>
+      <c r="F2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="41" t="s">
+      <c r="G2" s="52"/>
+      <c r="H2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="44" t="s">
+      <c r="I2" s="53"/>
+      <c r="J2" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="56"/>
+    </row>
+    <row r="3" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="38"/>
-    </row>
-    <row r="3" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="45"/>
-    </row>
-    <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="46" t="s">
+      <c r="C4" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="39" t="str">
+        <f>IF(EXACT(K4,""),"", IF(K4&lt;$M$4, "Existe Relación Lineal Significante", "No Existe Relación Lineal Significante"))</f>
+        <v/>
+      </c>
+      <c r="M4" s="37">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="48"/>
+      <c r="C5" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="50"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="47"/>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="49"/>
+      <c r="C6" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="51"/>
-    </row>
-    <row r="6" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="48"/>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="39" t="str">
+        <f t="shared" ref="L7" si="0">IF(EXACT(K7,""),"", IF(K7&lt;$M$4, "Existe Relación Lineal Significante", "No Existe Relación Lineal Significante"))</f>
+        <v/>
+      </c>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="48"/>
+      <c r="C8" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="49"/>
+      <c r="C9" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="39" t="str">
+        <f t="shared" ref="L10" si="1">IF(EXACT(K10,""),"", IF(K10&lt;$M$4, "Existe Relación Lineal Significante", "No Existe Relación Lineal Significante"))</f>
+        <v/>
+      </c>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="48"/>
+      <c r="C11" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="50"/>
+      <c r="C12" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="10"/>
+    </row>
+    <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="39" t="str">
+        <f t="shared" ref="L13" si="2">IF(EXACT(K13,""),"", IF(K13&lt;$M$4, "Existe Relación Lineal Significante", "No Existe Relación Lineal Significante"))</f>
+        <v/>
+      </c>
+      <c r="M13" s="35"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="48"/>
+      <c r="C14" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="50"/>
+      <c r="C15" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="51"/>
-    </row>
-    <row r="7" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="46" t="s">
+      <c r="D16" s="22">
+        <f t="shared" ref="D16:I18" si="3">SUM(D4,D7,D10,D13)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="50"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="47"/>
-      <c r="C8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="51"/>
-    </row>
-    <row r="9" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="48"/>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="51"/>
-    </row>
-    <row r="10" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="46" t="s">
+      <c r="D17" s="23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="50"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="47"/>
-      <c r="C11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="51"/>
-    </row>
-    <row r="12" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="49"/>
-      <c r="C12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="51"/>
-    </row>
-    <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="46" t="s">
+      <c r="D18" s="31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="50"/>
-      <c r="M13" s="52"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="47"/>
-      <c r="C14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="51"/>
-    </row>
-    <row r="15" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="49"/>
-      <c r="C15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="39"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C16" s="9" t="s">
+      <c r="D19" s="22" t="e">
+        <f t="shared" ref="D19:I21" si="4">STDEVA(D4,D7,D10,D13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E19" s="25" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F19" s="25" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" s="28" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="25" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="26">
-        <f t="shared" ref="D16:I18" si="0">SUM(D4,D7,D10,D13)</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C17" s="10" t="s">
+      <c r="D20" s="23" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E20" s="26" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F20" s="26" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G20" s="29" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="23" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" s="26" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C19" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="26" t="e">
-        <f t="shared" ref="D19:I21" si="1">STDEVA(D4,D7,D10,D13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E19" s="29" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F19" s="29" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G19" s="32" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H19" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" s="29" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="27" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E20" s="30" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F20" s="30" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G20" s="33" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H20" s="27" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I20" s="30" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="3:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="28" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E21" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F21" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G21" s="34" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H21" s="28" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I21" s="31" t="e">
-        <f t="shared" si="1"/>
+      <c r="D21" s="24" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E21" s="27" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F21" s="27" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" s="30" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="24" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" s="27" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
   </mergeCells>
+  <conditionalFormatting sqref="L4 L7 L10 L13">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",L4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Existe Relación Lineal Significante">
+      <formula>NOT(ISERROR(SEARCH("Existe Relación Lineal Significante",L4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="No Existe Relación Lineal Significante">
+      <formula>NOT(ISERROR(SEARCH("No Existe Relación Lineal Significante",L4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Existe Relación Lineal Significante">
+      <formula>NOT(ISERROR(SEARCH("Existe Relación Lineal Significante",L4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5 L8 L11 L14">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="No Existe Relación Lineal Significante">
+      <formula>NOT(ISERROR(SEARCH("No Existe Relación Lineal Significante",L5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>